<commit_message>
Changed 2 lines of code around 1212 of uot tool and initial test seesm successful.
</commit_message>
<xml_diff>
--- a/autoast/auto_ast_V2_Cuisinart_MultiP_PdfMaps/jobs.xlsx
+++ b/autoast/auto_ast_V2_Cuisinart_MultiP_PdfMaps/jobs.xlsx
@@ -45,9 +45,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="1" xfId="0">
       <alignment horizontal="general"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -426,139 +429,139 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
-    <col width="51.29071428571429" bestFit="1" customWidth="1" style="2" min="1" max="1"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="2" min="2" max="2"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="2" min="3" max="3"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="2" min="4" max="4"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="2" min="5" max="5"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="2" min="6" max="6"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="2" min="7" max="7"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="2" min="8" max="8"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="2" min="9" max="9"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="2" min="10" max="10"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="2" min="11" max="11"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="2" min="12" max="12"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="2" min="13" max="13"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="2" min="14" max="14"/>
+    <col width="51.29071428571429" bestFit="1" customWidth="1" style="3" min="1" max="1"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="3" min="2" max="2"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="3" min="3" max="3"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="3" min="4" max="4"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="3" min="5" max="5"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="3" min="6" max="6"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="3" min="7" max="7"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="3" min="8" max="8"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="3" min="9" max="9"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="3" min="10" max="10"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="3" min="11" max="11"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="3" min="12" max="12"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="3" min="13" max="13"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="3" min="14" max="14"/>
   </cols>
   <sheetData>
     <row r="1" ht="18.75" customHeight="1">
-      <c r="A1" s="2" t="inlineStr">
+      <c r="A1" s="3" t="inlineStr">
         <is>
           <t>region</t>
         </is>
       </c>
-      <c r="B1" s="2" t="inlineStr">
+      <c r="B1" s="3" t="inlineStr">
         <is>
           <t>feature_layer</t>
         </is>
       </c>
-      <c r="C1" s="2" t="inlineStr">
+      <c r="C1" s="3" t="inlineStr">
         <is>
           <t>crown_file_number</t>
         </is>
       </c>
-      <c r="D1" s="2" t="inlineStr">
+      <c r="D1" s="3" t="inlineStr">
         <is>
           <t>disposition_number</t>
         </is>
       </c>
-      <c r="E1" s="2" t="inlineStr">
+      <c r="E1" s="3" t="inlineStr">
         <is>
           <t>parcel_number</t>
         </is>
       </c>
-      <c r="F1" s="2" t="inlineStr">
+      <c r="F1" s="3" t="inlineStr">
         <is>
           <t>output_directory</t>
         </is>
       </c>
-      <c r="G1" s="2" t="inlineStr">
+      <c r="G1" s="3" t="inlineStr">
         <is>
           <t>output_directory_same_as_input</t>
         </is>
       </c>
-      <c r="H1" s="2" t="inlineStr">
+      <c r="H1" s="3" t="inlineStr">
         <is>
           <t>dont_overwrite_outputs</t>
         </is>
       </c>
-      <c r="I1" s="2" t="inlineStr">
+      <c r="I1" s="3" t="inlineStr">
         <is>
           <t>skip_conflicts_and_constraints</t>
         </is>
       </c>
-      <c r="J1" s="2" t="inlineStr">
+      <c r="J1" s="3" t="inlineStr">
         <is>
           <t>suppress_map_creation</t>
         </is>
       </c>
-      <c r="K1" s="2" t="inlineStr">
+      <c r="K1" s="3" t="inlineStr">
         <is>
           <t>add_maps_to_current</t>
         </is>
       </c>
-      <c r="L1" s="2" t="inlineStr">
+      <c r="L1" s="3" t="inlineStr">
         <is>
           <t>run_as_fcbc</t>
         </is>
       </c>
-      <c r="M1" s="2" t="inlineStr">
+      <c r="M1" s="3" t="inlineStr">
         <is>
           <t>ast_condition</t>
         </is>
       </c>
-      <c r="N1" s="2" t="inlineStr">
+      <c r="N1" s="3" t="inlineStr">
         <is>
           <t>file_number</t>
         </is>
       </c>
     </row>
     <row r="2" ht="18.75" customHeight="1">
-      <c r="A2" s="2" t="inlineStr">
+      <c r="A2" s="3" t="inlineStr">
         <is>
           <t>Thompson_Okanagan</t>
         </is>
       </c>
-      <c r="B2" s="2" t="inlineStr">
+      <c r="B2" s="3" t="inlineStr">
         <is>
           <t>//spatialfiles.bcgov/work/srm/nel/Local/Geomatics/Workarea/csostad/Statusing/test\Boulder &amp; Elkhart\Boulder &amp; Elkhart.shp</t>
         </is>
       </c>
-      <c r="C2" s="2" t="n"/>
-      <c r="D2" s="2" t="n"/>
-      <c r="E2" s="2" t="n"/>
-      <c r="F2" s="2" t="inlineStr">
+      <c r="C2" s="3" t="n"/>
+      <c r="D2" s="3" t="n"/>
+      <c r="E2" s="3" t="n"/>
+      <c r="F2" s="3" t="inlineStr">
         <is>
           <t>//spatialfiles.bcgov/work/srm/nel/Local/Geomatics/Workarea/csostad/Statusing/test\outputs\Boulder &amp; Elkhart</t>
         </is>
       </c>
-      <c r="G2" s="2" t="inlineStr">
-        <is>
-          <t>false</t>
-        </is>
-      </c>
-      <c r="H2" s="2" t="inlineStr">
-        <is>
-          <t>false</t>
-        </is>
-      </c>
-      <c r="I2" s="2" t="inlineStr">
-        <is>
-          <t>false</t>
-        </is>
-      </c>
-      <c r="J2" s="2" t="inlineStr">
-        <is>
-          <t>false</t>
-        </is>
-      </c>
-      <c r="K2" s="2" t="inlineStr">
-        <is>
-          <t>false</t>
-        </is>
-      </c>
-      <c r="L2" s="2" t="inlineStr">
+      <c r="G2" s="3" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+      <c r="H2" s="3" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+      <c r="I2" s="3" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+      <c r="J2" s="3" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+      <c r="K2" s="3" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+      <c r="L2" s="3" t="inlineStr">
         <is>
           <t>true</t>
         </is>
@@ -568,53 +571,53 @@
           <t>COMPLETE</t>
         </is>
       </c>
-      <c r="N2" s="2" t="n"/>
+      <c r="N2" s="3" t="n"/>
     </row>
     <row r="3" ht="18.75" customHeight="1">
-      <c r="A3" s="2" t="inlineStr">
+      <c r="A3" s="3" t="inlineStr">
         <is>
           <t>Thompson_Okanagan</t>
         </is>
       </c>
-      <c r="B3" s="2" t="inlineStr">
+      <c r="B3" s="3" t="inlineStr">
         <is>
           <t>//spatialfiles.bcgov/work/srm/nel/Local/Geomatics/Workarea/csostad/Statusing/test\Brewster\Brewster.shp</t>
         </is>
       </c>
-      <c r="C3" s="2" t="n"/>
-      <c r="D3" s="2" t="n"/>
-      <c r="E3" s="2" t="n"/>
-      <c r="F3" s="2" t="inlineStr">
+      <c r="C3" s="3" t="n"/>
+      <c r="D3" s="3" t="n"/>
+      <c r="E3" s="3" t="n"/>
+      <c r="F3" s="3" t="inlineStr">
         <is>
           <t>//spatialfiles.bcgov/work/srm/nel/Local/Geomatics/Workarea/csostad/Statusing/test\outputs\Brewster</t>
         </is>
       </c>
-      <c r="G3" s="2" t="inlineStr">
-        <is>
-          <t>false</t>
-        </is>
-      </c>
-      <c r="H3" s="2" t="inlineStr">
-        <is>
-          <t>false</t>
-        </is>
-      </c>
-      <c r="I3" s="2" t="inlineStr">
-        <is>
-          <t>false</t>
-        </is>
-      </c>
-      <c r="J3" s="2" t="inlineStr">
-        <is>
-          <t>false</t>
-        </is>
-      </c>
-      <c r="K3" s="2" t="inlineStr">
-        <is>
-          <t>false</t>
-        </is>
-      </c>
-      <c r="L3" s="2" t="inlineStr">
+      <c r="G3" s="3" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+      <c r="H3" s="3" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+      <c r="I3" s="3" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+      <c r="J3" s="3" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+      <c r="K3" s="3" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+      <c r="L3" s="3" t="inlineStr">
         <is>
           <t>true</t>
         </is>
@@ -624,7 +627,7 @@
           <t>COMPLETE</t>
         </is>
       </c>
-      <c r="N3" s="2" t="n"/>
+      <c r="N3" s="3" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>